<commit_message>
Implement scripts for another speedway programs
</commit_message>
<xml_diff>
--- a/dist/ekstraliga.xlsx
+++ b/dist/ekstraliga.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aland\Desktop\exceljs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aland\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA49F6A6-B2E0-4A96-96BC-E9DCA49985AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB29FE0-319E-4164-8A22-837D8E757B92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="510" yWindow="810" windowWidth="19860" windowHeight="6840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$zł-415];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$zł-415]"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -629,15 +629,6 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Black"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -1553,7 +1544,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1714,6 +1705,75 @@
     <xf numFmtId="16" fontId="15" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1747,88 +1807,7 @@
     <xf numFmtId="0" fontId="11" fillId="13" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Graphics" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2012,23 +1991,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Obraz 10">
+        <xdr:cNvPr id="4" name="Obraz 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{385B71D3-1A22-4B18-9766-4C97C23E1318}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85BBA172-7E1F-4F4D-AC72-EBA4CA230D7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2037,7 +2016,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2050,8 +2029,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7905750" y="6105525"/>
-          <a:ext cx="400050" cy="400050"/>
+          <a:off x="6572251" y="6076950"/>
+          <a:ext cx="1162049" cy="406400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2062,23 +2041,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>169049</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>121424</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:rowOff>48744</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Obraz 14">
+        <xdr:cNvPr id="6" name="Obraz 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73AD0125-58E5-4A69-A5B6-1BB71136E7A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{665E5429-72A8-4866-B853-C2D9A57DAB3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2087,7 +2066,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2100,308 +2079,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8465324" y="6065024"/>
-          <a:ext cx="488175" cy="488175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>480975</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>138075</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>923925</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Obraz 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC903A1-CF81-45F7-9F2E-8888DC1B1BCC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7291350" y="6081675"/>
-          <a:ext cx="442950" cy="442950"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>97575</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>154725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Obraz 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF2F9232-8A68-48B0-8C3D-6C3EEAF52E9F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9679725" y="6098325"/>
-          <a:ext cx="445350" cy="445350"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>447599</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>152324</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Obraz 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84E3248A-F935-4BB1-A687-CC1E5F0A77B9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10296449" y="6095924"/>
-          <a:ext cx="457275" cy="457275"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>35624</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>149924</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Obraz 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{972504D6-2FCA-427D-A978-3B8DB4082E38}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9103424" y="6093524"/>
-          <a:ext cx="459675" cy="459675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>90374</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>52274</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Obraz 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A6D6FDC-92EC-46D9-B01B-7F7A8F03EA03}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5891099" y="5995874"/>
-          <a:ext cx="595425" cy="595425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>68941</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>68941</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Obraz 26">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEA32E7F-7B36-4176-9191-C49EE14ACD4B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6574516" y="6012541"/>
-          <a:ext cx="559709" cy="559709"/>
+          <a:off x="7915275" y="6048375"/>
+          <a:ext cx="2571750" cy="429744"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2736,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AI53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AN38" sqref="AN38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2804,87 +2483,87 @@
       <c r="AI1" s="1"/>
     </row>
     <row r="2" spans="2:35" ht="14.25" customHeight="1">
-      <c r="B2" s="108"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="113"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="106"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="108"/>
-      <c r="U2" s="74"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="74"/>
-      <c r="X2" s="74"/>
-      <c r="Y2" s="74"/>
-      <c r="Z2" s="74"/>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="74"/>
-      <c r="AC2" s="74"/>
-      <c r="AD2" s="74"/>
-      <c r="AE2" s="74"/>
-      <c r="AF2" s="74"/>
-      <c r="AG2" s="74"/>
-      <c r="AH2" s="75"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105"/>
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
+      <c r="AB2" s="105"/>
+      <c r="AC2" s="105"/>
+      <c r="AD2" s="105"/>
+      <c r="AE2" s="105"/>
+      <c r="AF2" s="105"/>
+      <c r="AG2" s="105"/>
+      <c r="AH2" s="106"/>
       <c r="AI2" s="1"/>
     </row>
     <row r="3" spans="2:35" ht="14.25" customHeight="1">
-      <c r="B3" s="109"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="115"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
+      <c r="N3" s="107"/>
+      <c r="O3" s="108"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="1"/>
       <c r="S3" s="58"/>
-      <c r="T3" s="109"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="76"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="76"/>
-      <c r="AA3" s="76"/>
-      <c r="AB3" s="76"/>
-      <c r="AC3" s="76"/>
-      <c r="AD3" s="76"/>
-      <c r="AE3" s="76"/>
-      <c r="AF3" s="76"/>
-      <c r="AG3" s="76"/>
-      <c r="AH3" s="77"/>
+      <c r="T3" s="79"/>
+      <c r="U3" s="107"/>
+      <c r="V3" s="107"/>
+      <c r="W3" s="107"/>
+      <c r="X3" s="107"/>
+      <c r="Y3" s="107"/>
+      <c r="Z3" s="107"/>
+      <c r="AA3" s="107"/>
+      <c r="AB3" s="107"/>
+      <c r="AC3" s="107"/>
+      <c r="AD3" s="107"/>
+      <c r="AE3" s="107"/>
+      <c r="AF3" s="107"/>
+      <c r="AG3" s="107"/>
+      <c r="AH3" s="108"/>
       <c r="AI3" s="1"/>
     </row>
     <row r="4" spans="2:35" ht="15">
       <c r="B4" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
       <c r="G4" s="66">
         <v>1</v>
       </c>
@@ -2915,12 +2594,12 @@
       <c r="T4" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="U4" s="119" t="s">
+      <c r="U4" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="V4" s="119"/>
-      <c r="W4" s="119"/>
-      <c r="X4" s="119"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
       <c r="Y4" s="66">
         <v>1</v>
       </c>
@@ -2953,10 +2632,10 @@
       <c r="B5" s="2">
         <v>9</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
       <c r="G5" s="3"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -2973,10 +2652,10 @@
       <c r="T5" s="2">
         <v>1</v>
       </c>
-      <c r="U5" s="110"/>
-      <c r="V5" s="110"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="110"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="4"/>
@@ -2993,10 +2672,10 @@
       <c r="B6" s="6">
         <v>10</v>
       </c>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -3013,10 +2692,10 @@
       <c r="T6" s="6">
         <v>2</v>
       </c>
-      <c r="U6" s="111"/>
-      <c r="V6" s="111"/>
-      <c r="W6" s="111"/>
-      <c r="X6" s="111"/>
+      <c r="U6" s="75"/>
+      <c r="V6" s="75"/>
+      <c r="W6" s="75"/>
+      <c r="X6" s="75"/>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
       <c r="AA6" s="8"/>
@@ -3033,10 +2712,10 @@
       <c r="B7" s="6">
         <v>11</v>
       </c>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -3052,10 +2731,10 @@
       <c r="T7" s="6">
         <v>3</v>
       </c>
-      <c r="U7" s="111"/>
-      <c r="V7" s="111"/>
-      <c r="W7" s="111"/>
-      <c r="X7" s="111"/>
+      <c r="U7" s="75"/>
+      <c r="V7" s="75"/>
+      <c r="W7" s="75"/>
+      <c r="X7" s="75"/>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="8"/>
@@ -3072,10 +2751,10 @@
       <c r="B8" s="6">
         <v>12</v>
       </c>
-      <c r="C8" s="111"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="111"/>
-      <c r="F8" s="111"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -3092,10 +2771,10 @@
       <c r="T8" s="6">
         <v>4</v>
       </c>
-      <c r="U8" s="111"/>
-      <c r="V8" s="111"/>
-      <c r="W8" s="111"/>
-      <c r="X8" s="111"/>
+      <c r="U8" s="75"/>
+      <c r="V8" s="75"/>
+      <c r="W8" s="75"/>
+      <c r="X8" s="75"/>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
       <c r="AA8" s="8"/>
@@ -3112,10 +2791,10 @@
       <c r="B9" s="6">
         <v>13</v>
       </c>
-      <c r="C9" s="111"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="111"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -3132,10 +2811,10 @@
       <c r="T9" s="6">
         <v>5</v>
       </c>
-      <c r="U9" s="111"/>
-      <c r="V9" s="111"/>
-      <c r="W9" s="111"/>
-      <c r="X9" s="111"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
+      <c r="X9" s="75"/>
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="8"/>
@@ -3152,10 +2831,10 @@
       <c r="B10" s="6">
         <v>14</v>
       </c>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="111"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -3172,10 +2851,10 @@
       <c r="T10" s="6">
         <v>6</v>
       </c>
-      <c r="U10" s="111"/>
-      <c r="V10" s="111"/>
-      <c r="W10" s="111"/>
-      <c r="X10" s="111"/>
+      <c r="U10" s="75"/>
+      <c r="V10" s="75"/>
+      <c r="W10" s="75"/>
+      <c r="X10" s="75"/>
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="8"/>
@@ -3192,10 +2871,10 @@
       <c r="B11" s="9">
         <v>15</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="104"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="90"/>
       <c r="G11" s="10"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -3212,10 +2891,10 @@
       <c r="T11" s="9">
         <v>7</v>
       </c>
-      <c r="U11" s="102"/>
-      <c r="V11" s="103"/>
-      <c r="W11" s="103"/>
-      <c r="X11" s="104"/>
+      <c r="U11" s="88"/>
+      <c r="V11" s="89"/>
+      <c r="W11" s="89"/>
+      <c r="X11" s="90"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
       <c r="AA11" s="11"/>
@@ -3232,10 +2911,10 @@
       <c r="B12" s="9">
         <v>16</v>
       </c>
-      <c r="C12" s="116"/>
-      <c r="D12" s="117"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="118"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="87"/>
       <c r="G12" s="10"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -3252,10 +2931,10 @@
       <c r="T12" s="9">
         <v>8</v>
       </c>
-      <c r="U12" s="120"/>
-      <c r="V12" s="120"/>
-      <c r="W12" s="120"/>
-      <c r="X12" s="120"/>
+      <c r="U12" s="77"/>
+      <c r="V12" s="77"/>
+      <c r="W12" s="77"/>
+      <c r="X12" s="77"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
       <c r="AA12" s="11"/>
@@ -3269,42 +2948,42 @@
       <c r="AI12" s="1"/>
     </row>
     <row r="13" spans="2:35" ht="15.75" thickBot="1">
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="80"/>
-      <c r="N13" s="81"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="112"/>
       <c r="O13" s="63"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="82" t="s">
+      <c r="T13" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="U13" s="83"/>
-      <c r="V13" s="83"/>
-      <c r="W13" s="83"/>
-      <c r="X13" s="83"/>
-      <c r="Y13" s="83"/>
-      <c r="Z13" s="83"/>
-      <c r="AA13" s="83"/>
-      <c r="AB13" s="83"/>
-      <c r="AC13" s="83"/>
-      <c r="AD13" s="83"/>
-      <c r="AE13" s="83"/>
-      <c r="AF13" s="83"/>
-      <c r="AG13" s="84"/>
+      <c r="U13" s="114"/>
+      <c r="V13" s="114"/>
+      <c r="W13" s="114"/>
+      <c r="X13" s="114"/>
+      <c r="Y13" s="114"/>
+      <c r="Z13" s="114"/>
+      <c r="AA13" s="114"/>
+      <c r="AB13" s="114"/>
+      <c r="AC13" s="114"/>
+      <c r="AD13" s="114"/>
+      <c r="AE13" s="114"/>
+      <c r="AF13" s="114"/>
+      <c r="AG13" s="115"/>
       <c r="AH13" s="63"/>
       <c r="AI13" s="1"/>
     </row>
@@ -3354,20 +3033,20 @@
       <c r="D15" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="105" t="s">
+      <c r="E15" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="105"/>
+      <c r="F15" s="93"/>
       <c r="G15" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="106" t="s">
+      <c r="H15" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="106"/>
-      <c r="J15" s="106"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="106"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
       <c r="M15" s="64" t="s">
         <v>10</v>
       </c>
@@ -3392,23 +3071,23 @@
       <c r="V15" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="W15" s="105" t="s">
+      <c r="W15" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="X15" s="105"/>
+      <c r="X15" s="93"/>
       <c r="Y15" s="65" t="s">
         <v>0</v>
       </c>
       <c r="Z15" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="AA15" s="106" t="s">
+      <c r="AA15" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="AB15" s="106"/>
-      <c r="AC15" s="106"/>
-      <c r="AD15" s="106"/>
-      <c r="AE15" s="106"/>
+      <c r="AB15" s="94"/>
+      <c r="AC15" s="94"/>
+      <c r="AD15" s="94"/>
+      <c r="AE15" s="94"/>
       <c r="AF15" s="64" t="s">
         <v>10</v>
       </c>
@@ -3423,7 +3102,7 @@
       </c>
     </row>
     <row r="16" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B16" s="95">
+      <c r="B16" s="80">
         <v>1</v>
       </c>
       <c r="C16" s="13" t="s">
@@ -3432,27 +3111,27 @@
       <c r="D16" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="96">
+      <c r="E16" s="81">
         <f>U5</f>
         <v>0</v>
       </c>
-      <c r="F16" s="96"/>
+      <c r="F16" s="81"/>
       <c r="G16" s="15">
         <v>1</v>
       </c>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="92"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="82"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="82"/>
       <c r="M16" s="16"/>
       <c r="N16" s="17"/>
-      <c r="O16" s="93"/>
-      <c r="P16" s="93"/>
+      <c r="O16" s="83"/>
+      <c r="P16" s="83"/>
       <c r="Q16" s="53"/>
-      <c r="R16" s="107"/>
+      <c r="R16" s="95"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="95">
+      <c r="T16" s="80">
         <v>9</v>
       </c>
       <c r="U16" s="13" t="s">
@@ -3461,138 +3140,138 @@
       <c r="V16" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W16" s="96">
+      <c r="W16" s="81">
         <f>U8</f>
         <v>0</v>
       </c>
-      <c r="X16" s="96"/>
+      <c r="X16" s="81"/>
       <c r="Y16" s="15">
         <v>1</v>
       </c>
       <c r="Z16" s="19">
         <v>4</v>
       </c>
-      <c r="AA16" s="92"/>
-      <c r="AB16" s="92"/>
-      <c r="AC16" s="92"/>
-      <c r="AD16" s="92"/>
-      <c r="AE16" s="92"/>
+      <c r="AA16" s="82"/>
+      <c r="AB16" s="82"/>
+      <c r="AC16" s="82"/>
+      <c r="AD16" s="82"/>
+      <c r="AE16" s="82"/>
       <c r="AF16" s="16"/>
       <c r="AG16" s="17"/>
-      <c r="AH16" s="93"/>
-      <c r="AI16" s="93"/>
+      <c r="AH16" s="83"/>
+      <c r="AI16" s="83"/>
     </row>
     <row r="17" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B17" s="95"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="94">
+      <c r="E17" s="91">
         <f>C5</f>
         <v>0</v>
       </c>
-      <c r="F17" s="94"/>
+      <c r="F17" s="91"/>
       <c r="G17" s="22">
         <v>9</v>
       </c>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="86"/>
-      <c r="L17" s="86"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
       <c r="M17" s="23"/>
       <c r="N17" s="24"/>
-      <c r="O17" s="93"/>
-      <c r="P17" s="93"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="83"/>
       <c r="Q17" s="53"/>
-      <c r="R17" s="107"/>
+      <c r="R17" s="95"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="95"/>
+      <c r="T17" s="80"/>
       <c r="U17" s="20" t="s">
         <v>2</v>
       </c>
       <c r="V17" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="W17" s="94">
+      <c r="W17" s="91">
         <f>C6</f>
         <v>0</v>
       </c>
-      <c r="X17" s="94"/>
+      <c r="X17" s="91"/>
       <c r="Y17" s="22">
         <v>9</v>
       </c>
       <c r="Z17" s="25">
         <v>10</v>
       </c>
-      <c r="AA17" s="86"/>
-      <c r="AB17" s="86"/>
-      <c r="AC17" s="86"/>
-      <c r="AD17" s="86"/>
-      <c r="AE17" s="86"/>
+      <c r="AA17" s="92"/>
+      <c r="AB17" s="92"/>
+      <c r="AC17" s="92"/>
+      <c r="AD17" s="92"/>
+      <c r="AE17" s="92"/>
       <c r="AF17" s="23"/>
       <c r="AG17" s="24"/>
-      <c r="AH17" s="93"/>
-      <c r="AI17" s="93"/>
+      <c r="AH17" s="83"/>
+      <c r="AI17" s="83"/>
     </row>
     <row r="18" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B18" s="95"/>
+      <c r="B18" s="80"/>
       <c r="C18" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="94">
+      <c r="E18" s="91">
         <f>U6</f>
         <v>0</v>
       </c>
-      <c r="F18" s="94"/>
+      <c r="F18" s="91"/>
       <c r="G18" s="26">
         <v>2</v>
       </c>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
-      <c r="L18" s="86"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="92"/>
       <c r="M18" s="23"/>
       <c r="N18" s="24"/>
-      <c r="O18" s="98"/>
-      <c r="P18" s="98"/>
+      <c r="O18" s="84"/>
+      <c r="P18" s="84"/>
       <c r="Q18" s="53"/>
-      <c r="R18" s="107"/>
+      <c r="R18" s="95"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="95"/>
+      <c r="T18" s="80"/>
       <c r="U18" s="20" t="s">
         <v>14</v>
       </c>
       <c r="V18" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="W18" s="94">
+      <c r="W18" s="91">
         <f>U7</f>
         <v>0</v>
       </c>
-      <c r="X18" s="94"/>
+      <c r="X18" s="91"/>
       <c r="Y18" s="26">
         <v>2</v>
       </c>
       <c r="Z18" s="27">
         <v>3</v>
       </c>
-      <c r="AA18" s="86"/>
-      <c r="AB18" s="86"/>
-      <c r="AC18" s="86"/>
-      <c r="AD18" s="86"/>
-      <c r="AE18" s="86"/>
+      <c r="AA18" s="92"/>
+      <c r="AB18" s="92"/>
+      <c r="AC18" s="92"/>
+      <c r="AD18" s="92"/>
+      <c r="AE18" s="92"/>
       <c r="AF18" s="23"/>
       <c r="AG18" s="24"/>
-      <c r="AH18" s="98"/>
-      <c r="AI18" s="98"/>
+      <c r="AH18" s="84"/>
+      <c r="AI18" s="84"/>
     </row>
     <row r="19" spans="2:35" ht="13.5" customHeight="1">
       <c r="B19" s="28"/>
@@ -3602,25 +3281,25 @@
       <c r="D19" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="88">
+      <c r="E19" s="96">
         <f>C6</f>
         <v>0</v>
       </c>
-      <c r="F19" s="88"/>
+      <c r="F19" s="96"/>
       <c r="G19" s="31">
         <v>10</v>
       </c>
-      <c r="H19" s="89"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="89"/>
-      <c r="K19" s="89"/>
-      <c r="L19" s="89"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="97"/>
       <c r="M19" s="32"/>
       <c r="N19" s="33"/>
-      <c r="O19" s="98"/>
-      <c r="P19" s="98"/>
+      <c r="O19" s="84"/>
+      <c r="P19" s="84"/>
       <c r="Q19" s="53"/>
-      <c r="R19" s="107"/>
+      <c r="R19" s="95"/>
       <c r="S19" s="1"/>
       <c r="T19" s="28"/>
       <c r="U19" s="29" t="s">
@@ -3629,29 +3308,29 @@
       <c r="V19" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="W19" s="88">
+      <c r="W19" s="96">
         <f>C5</f>
         <v>0</v>
       </c>
-      <c r="X19" s="88"/>
+      <c r="X19" s="96"/>
       <c r="Y19" s="31">
         <v>10</v>
       </c>
       <c r="Z19" s="34">
         <v>9</v>
       </c>
-      <c r="AA19" s="89"/>
-      <c r="AB19" s="89"/>
-      <c r="AC19" s="89"/>
-      <c r="AD19" s="89"/>
-      <c r="AE19" s="89"/>
+      <c r="AA19" s="97"/>
+      <c r="AB19" s="97"/>
+      <c r="AC19" s="97"/>
+      <c r="AD19" s="97"/>
+      <c r="AE19" s="97"/>
       <c r="AF19" s="32"/>
       <c r="AG19" s="33"/>
-      <c r="AH19" s="98"/>
-      <c r="AI19" s="98"/>
+      <c r="AH19" s="84"/>
+      <c r="AI19" s="84"/>
     </row>
     <row r="20" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B20" s="95">
+      <c r="B20" s="80">
         <v>2</v>
       </c>
       <c r="C20" s="13" t="s">
@@ -3660,27 +3339,27 @@
       <c r="D20" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="101">
+      <c r="E20" s="98">
         <f>C11</f>
         <v>0</v>
       </c>
-      <c r="F20" s="101"/>
+      <c r="F20" s="98"/>
       <c r="G20" s="35">
         <v>15</v>
       </c>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="92"/>
-      <c r="L20" s="92"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="82"/>
       <c r="M20" s="16"/>
       <c r="N20" s="17"/>
-      <c r="O20" s="93"/>
-      <c r="P20" s="93"/>
+      <c r="O20" s="83"/>
+      <c r="P20" s="83"/>
       <c r="Q20" s="53"/>
-      <c r="R20" s="107"/>
+      <c r="R20" s="95"/>
       <c r="S20" s="1"/>
-      <c r="T20" s="95">
+      <c r="T20" s="80">
         <v>10</v>
       </c>
       <c r="U20" s="13" t="s">
@@ -3689,138 +3368,138 @@
       <c r="V20" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W20" s="96">
+      <c r="W20" s="81">
         <f>U11</f>
         <v>0</v>
       </c>
-      <c r="X20" s="96"/>
+      <c r="X20" s="81"/>
       <c r="Y20" s="15">
         <v>1</v>
       </c>
       <c r="Z20" s="36">
         <v>7</v>
       </c>
-      <c r="AA20" s="92"/>
-      <c r="AB20" s="92"/>
-      <c r="AC20" s="92"/>
-      <c r="AD20" s="92"/>
-      <c r="AE20" s="92"/>
+      <c r="AA20" s="82"/>
+      <c r="AB20" s="82"/>
+      <c r="AC20" s="82"/>
+      <c r="AD20" s="82"/>
+      <c r="AE20" s="82"/>
       <c r="AF20" s="16"/>
       <c r="AG20" s="17"/>
-      <c r="AH20" s="93"/>
-      <c r="AI20" s="93"/>
+      <c r="AH20" s="83"/>
+      <c r="AI20" s="83"/>
     </row>
     <row r="21" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B21" s="95"/>
+      <c r="B21" s="80"/>
       <c r="C21" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="94">
+      <c r="E21" s="91">
         <f>U10</f>
         <v>0</v>
       </c>
-      <c r="F21" s="94"/>
+      <c r="F21" s="91"/>
       <c r="G21" s="27">
         <v>6</v>
       </c>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="86"/>
-      <c r="K21" s="86"/>
-      <c r="L21" s="86"/>
+      <c r="H21" s="92"/>
+      <c r="I21" s="92"/>
+      <c r="J21" s="92"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="92"/>
       <c r="M21" s="23"/>
       <c r="N21" s="24"/>
-      <c r="O21" s="93"/>
-      <c r="P21" s="93"/>
+      <c r="O21" s="83"/>
+      <c r="P21" s="83"/>
       <c r="Q21" s="53"/>
-      <c r="R21" s="107"/>
+      <c r="R21" s="95"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="95"/>
+      <c r="T21" s="80"/>
       <c r="U21" s="20" t="s">
         <v>2</v>
       </c>
       <c r="V21" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="W21" s="94">
+      <c r="W21" s="91">
         <f>C7</f>
         <v>0</v>
       </c>
-      <c r="X21" s="94"/>
+      <c r="X21" s="91"/>
       <c r="Y21" s="22">
         <v>9</v>
       </c>
       <c r="Z21" s="22">
         <v>11</v>
       </c>
-      <c r="AA21" s="86"/>
-      <c r="AB21" s="86"/>
-      <c r="AC21" s="86"/>
-      <c r="AD21" s="86"/>
-      <c r="AE21" s="86"/>
+      <c r="AA21" s="92"/>
+      <c r="AB21" s="92"/>
+      <c r="AC21" s="92"/>
+      <c r="AD21" s="92"/>
+      <c r="AE21" s="92"/>
       <c r="AF21" s="23"/>
       <c r="AG21" s="24"/>
-      <c r="AH21" s="93"/>
-      <c r="AI21" s="93"/>
+      <c r="AH21" s="83"/>
+      <c r="AI21" s="83"/>
     </row>
     <row r="22" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B22" s="95"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="94">
+      <c r="E22" s="91">
         <f>C10</f>
         <v>0</v>
       </c>
-      <c r="F22" s="94"/>
+      <c r="F22" s="91"/>
       <c r="G22" s="22">
         <v>14</v>
       </c>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="86"/>
-      <c r="K22" s="86"/>
-      <c r="L22" s="86"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="92"/>
+      <c r="K22" s="92"/>
+      <c r="L22" s="92"/>
       <c r="M22" s="23"/>
       <c r="N22" s="24"/>
-      <c r="O22" s="98"/>
-      <c r="P22" s="98"/>
+      <c r="O22" s="84"/>
+      <c r="P22" s="84"/>
       <c r="Q22" s="53"/>
-      <c r="R22" s="107"/>
+      <c r="R22" s="95"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="95"/>
+      <c r="T22" s="80"/>
       <c r="U22" s="20" t="s">
         <v>14</v>
       </c>
       <c r="V22" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="W22" s="94">
+      <c r="W22" s="91">
         <f>U9</f>
         <v>0</v>
       </c>
-      <c r="X22" s="94"/>
+      <c r="X22" s="91"/>
       <c r="Y22" s="26">
         <v>2</v>
       </c>
       <c r="Z22" s="27">
         <v>5</v>
       </c>
-      <c r="AA22" s="86"/>
-      <c r="AB22" s="86"/>
-      <c r="AC22" s="86"/>
-      <c r="AD22" s="86"/>
-      <c r="AE22" s="86"/>
+      <c r="AA22" s="92"/>
+      <c r="AB22" s="92"/>
+      <c r="AC22" s="92"/>
+      <c r="AD22" s="92"/>
+      <c r="AE22" s="92"/>
       <c r="AF22" s="23"/>
       <c r="AG22" s="24"/>
-      <c r="AH22" s="98"/>
-      <c r="AI22" s="98"/>
+      <c r="AH22" s="84"/>
+      <c r="AI22" s="84"/>
     </row>
     <row r="23" spans="2:35" ht="13.5" customHeight="1">
       <c r="B23" s="28"/>
@@ -3830,25 +3509,25 @@
       <c r="D23" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="88">
+      <c r="E23" s="96">
         <f>U11</f>
         <v>0</v>
       </c>
-      <c r="F23" s="88"/>
+      <c r="F23" s="96"/>
       <c r="G23" s="37">
         <v>7</v>
       </c>
-      <c r="H23" s="89"/>
-      <c r="I23" s="89"/>
-      <c r="J23" s="89"/>
-      <c r="K23" s="89"/>
-      <c r="L23" s="89"/>
+      <c r="H23" s="97"/>
+      <c r="I23" s="97"/>
+      <c r="J23" s="97"/>
+      <c r="K23" s="97"/>
+      <c r="L23" s="97"/>
       <c r="M23" s="32"/>
       <c r="N23" s="33"/>
-      <c r="O23" s="98"/>
-      <c r="P23" s="98"/>
+      <c r="O23" s="84"/>
+      <c r="P23" s="84"/>
       <c r="Q23" s="53"/>
-      <c r="R23" s="107"/>
+      <c r="R23" s="95"/>
       <c r="S23" s="1"/>
       <c r="T23" s="28"/>
       <c r="U23" s="29" t="s">
@@ -3857,29 +3536,29 @@
       <c r="V23" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="W23" s="88">
+      <c r="W23" s="96">
         <f>C8</f>
         <v>0</v>
       </c>
-      <c r="X23" s="88"/>
+      <c r="X23" s="96"/>
       <c r="Y23" s="31">
         <v>10</v>
       </c>
       <c r="Z23" s="31">
         <v>12</v>
       </c>
-      <c r="AA23" s="89"/>
-      <c r="AB23" s="89"/>
-      <c r="AC23" s="89"/>
-      <c r="AD23" s="89"/>
-      <c r="AE23" s="89"/>
+      <c r="AA23" s="97"/>
+      <c r="AB23" s="97"/>
+      <c r="AC23" s="97"/>
+      <c r="AD23" s="97"/>
+      <c r="AE23" s="97"/>
       <c r="AF23" s="32"/>
       <c r="AG23" s="33"/>
-      <c r="AH23" s="98"/>
-      <c r="AI23" s="98"/>
+      <c r="AH23" s="84"/>
+      <c r="AI23" s="84"/>
     </row>
     <row r="24" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B24" s="95">
+      <c r="B24" s="80">
         <v>3</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -3888,27 +3567,27 @@
       <c r="D24" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="96">
+      <c r="E24" s="81">
         <f>C7</f>
         <v>0</v>
       </c>
-      <c r="F24" s="96"/>
+      <c r="F24" s="81"/>
       <c r="G24" s="38">
         <v>11</v>
       </c>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-      <c r="L24" s="92"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="82"/>
       <c r="M24" s="16"/>
       <c r="N24" s="17"/>
-      <c r="O24" s="93"/>
-      <c r="P24" s="93"/>
+      <c r="O24" s="83"/>
+      <c r="P24" s="83"/>
       <c r="Q24" s="53"/>
-      <c r="R24" s="107"/>
+      <c r="R24" s="95"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="95">
+      <c r="T24" s="80">
         <v>11</v>
       </c>
       <c r="U24" s="13" t="s">
@@ -3917,138 +3596,138 @@
       <c r="V24" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W24" s="96">
+      <c r="W24" s="81">
         <f>C6</f>
         <v>0</v>
       </c>
-      <c r="X24" s="96"/>
+      <c r="X24" s="81"/>
       <c r="Y24" s="15">
         <v>1</v>
       </c>
       <c r="Z24" s="35">
         <v>10</v>
       </c>
-      <c r="AA24" s="92"/>
-      <c r="AB24" s="92"/>
-      <c r="AC24" s="92"/>
-      <c r="AD24" s="92"/>
-      <c r="AE24" s="92"/>
+      <c r="AA24" s="82"/>
+      <c r="AB24" s="82"/>
+      <c r="AC24" s="82"/>
+      <c r="AD24" s="82"/>
+      <c r="AE24" s="82"/>
       <c r="AF24" s="16"/>
       <c r="AG24" s="17"/>
-      <c r="AH24" s="93"/>
-      <c r="AI24" s="93"/>
+      <c r="AH24" s="83"/>
+      <c r="AI24" s="83"/>
     </row>
     <row r="25" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B25" s="95"/>
+      <c r="B25" s="80"/>
       <c r="C25" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="94">
+      <c r="E25" s="91">
         <f>U7</f>
         <v>0</v>
       </c>
-      <c r="F25" s="94"/>
+      <c r="F25" s="91"/>
       <c r="G25" s="27">
         <v>3</v>
       </c>
-      <c r="H25" s="86"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="86"/>
-      <c r="K25" s="86"/>
-      <c r="L25" s="86"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="92"/>
       <c r="M25" s="23"/>
       <c r="N25" s="24"/>
-      <c r="O25" s="93"/>
-      <c r="P25" s="93"/>
+      <c r="O25" s="83"/>
+      <c r="P25" s="83"/>
       <c r="Q25" s="53"/>
-      <c r="R25" s="107"/>
+      <c r="R25" s="95"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="95"/>
+      <c r="T25" s="80"/>
       <c r="U25" s="20" t="s">
         <v>2</v>
       </c>
       <c r="V25" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="W25" s="94">
+      <c r="W25" s="91">
         <f>U6</f>
         <v>0</v>
       </c>
-      <c r="X25" s="94"/>
+      <c r="X25" s="91"/>
       <c r="Y25" s="22">
         <v>9</v>
       </c>
       <c r="Z25" s="39">
         <v>2</v>
       </c>
-      <c r="AA25" s="86"/>
-      <c r="AB25" s="86"/>
-      <c r="AC25" s="86"/>
-      <c r="AD25" s="86"/>
-      <c r="AE25" s="86"/>
+      <c r="AA25" s="92"/>
+      <c r="AB25" s="92"/>
+      <c r="AC25" s="92"/>
+      <c r="AD25" s="92"/>
+      <c r="AE25" s="92"/>
       <c r="AF25" s="23"/>
       <c r="AG25" s="24"/>
-      <c r="AH25" s="93"/>
-      <c r="AI25" s="93"/>
+      <c r="AH25" s="83"/>
+      <c r="AI25" s="83"/>
     </row>
     <row r="26" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B26" s="95"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="94">
+      <c r="E26" s="91">
         <f>C8</f>
         <v>0</v>
       </c>
-      <c r="F26" s="94"/>
+      <c r="F26" s="91"/>
       <c r="G26" s="25">
         <v>12</v>
       </c>
-      <c r="H26" s="86"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="86"/>
-      <c r="K26" s="86"/>
-      <c r="L26" s="86"/>
+      <c r="H26" s="92"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="92"/>
+      <c r="K26" s="92"/>
+      <c r="L26" s="92"/>
       <c r="M26" s="23"/>
       <c r="N26" s="24"/>
-      <c r="O26" s="98"/>
-      <c r="P26" s="98"/>
+      <c r="O26" s="84"/>
+      <c r="P26" s="84"/>
       <c r="Q26" s="53"/>
-      <c r="R26" s="107"/>
+      <c r="R26" s="95"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="95"/>
+      <c r="T26" s="80"/>
       <c r="U26" s="20" t="s">
         <v>14</v>
       </c>
       <c r="V26" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="W26" s="94">
+      <c r="W26" s="91">
         <f>C9</f>
         <v>0</v>
       </c>
-      <c r="X26" s="94"/>
+      <c r="X26" s="91"/>
       <c r="Y26" s="26">
         <v>2</v>
       </c>
       <c r="Z26" s="22">
         <v>13</v>
       </c>
-      <c r="AA26" s="86"/>
-      <c r="AB26" s="86"/>
-      <c r="AC26" s="86"/>
-      <c r="AD26" s="86"/>
-      <c r="AE26" s="86"/>
+      <c r="AA26" s="92"/>
+      <c r="AB26" s="92"/>
+      <c r="AC26" s="92"/>
+      <c r="AD26" s="92"/>
+      <c r="AE26" s="92"/>
       <c r="AF26" s="23"/>
       <c r="AG26" s="24"/>
-      <c r="AH26" s="98"/>
-      <c r="AI26" s="98"/>
+      <c r="AH26" s="84"/>
+      <c r="AI26" s="84"/>
     </row>
     <row r="27" spans="2:35" ht="13.5" customHeight="1">
       <c r="B27" s="28"/>
@@ -4058,25 +3737,25 @@
       <c r="D27" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="88">
+      <c r="E27" s="96">
         <f>U8</f>
         <v>0</v>
       </c>
-      <c r="F27" s="88"/>
+      <c r="F27" s="96"/>
       <c r="G27" s="37">
         <v>4</v>
       </c>
-      <c r="H27" s="89"/>
-      <c r="I27" s="89"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="89"/>
-      <c r="L27" s="89"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="97"/>
       <c r="M27" s="32"/>
       <c r="N27" s="33"/>
-      <c r="O27" s="98"/>
-      <c r="P27" s="98"/>
+      <c r="O27" s="84"/>
+      <c r="P27" s="84"/>
       <c r="Q27" s="53"/>
-      <c r="R27" s="107"/>
+      <c r="R27" s="95"/>
       <c r="S27" s="1"/>
       <c r="T27" s="28"/>
       <c r="U27" s="29" t="s">
@@ -4085,29 +3764,29 @@
       <c r="V27" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="W27" s="88">
+      <c r="W27" s="96">
         <f>U7</f>
         <v>0</v>
       </c>
-      <c r="X27" s="88"/>
+      <c r="X27" s="96"/>
       <c r="Y27" s="31">
         <v>10</v>
       </c>
       <c r="Z27" s="40">
         <v>3</v>
       </c>
-      <c r="AA27" s="89"/>
-      <c r="AB27" s="89"/>
-      <c r="AC27" s="89"/>
-      <c r="AD27" s="89"/>
-      <c r="AE27" s="89"/>
+      <c r="AA27" s="97"/>
+      <c r="AB27" s="97"/>
+      <c r="AC27" s="97"/>
+      <c r="AD27" s="97"/>
+      <c r="AE27" s="97"/>
       <c r="AF27" s="32"/>
       <c r="AG27" s="33"/>
-      <c r="AH27" s="98"/>
-      <c r="AI27" s="98"/>
+      <c r="AH27" s="84"/>
+      <c r="AI27" s="84"/>
     </row>
     <row r="28" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B28" s="95">
+      <c r="B28" s="80">
         <v>4</v>
       </c>
       <c r="C28" s="13" t="s">
@@ -4116,27 +3795,27 @@
       <c r="D28" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="96">
+      <c r="E28" s="81">
         <f>U9</f>
         <v>0</v>
       </c>
-      <c r="F28" s="96"/>
+      <c r="F28" s="81"/>
       <c r="G28" s="15">
         <v>5</v>
       </c>
-      <c r="H28" s="92"/>
-      <c r="I28" s="92"/>
-      <c r="J28" s="92"/>
-      <c r="K28" s="92"/>
-      <c r="L28" s="92"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
       <c r="M28" s="16"/>
       <c r="N28" s="17"/>
-      <c r="O28" s="93"/>
-      <c r="P28" s="93"/>
+      <c r="O28" s="83"/>
+      <c r="P28" s="83"/>
       <c r="Q28" s="53"/>
-      <c r="R28" s="107"/>
+      <c r="R28" s="95"/>
       <c r="S28" s="1"/>
-      <c r="T28" s="95">
+      <c r="T28" s="80">
         <v>12</v>
       </c>
       <c r="U28" s="13" t="s">
@@ -4145,138 +3824,138 @@
       <c r="V28" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W28" s="96">
+      <c r="W28" s="81">
         <f>U10</f>
         <v>0</v>
       </c>
-      <c r="X28" s="96"/>
+      <c r="X28" s="81"/>
       <c r="Y28" s="15">
         <v>1</v>
       </c>
       <c r="Z28" s="19">
         <v>6</v>
       </c>
-      <c r="AA28" s="92"/>
-      <c r="AB28" s="92"/>
-      <c r="AC28" s="92"/>
-      <c r="AD28" s="92"/>
-      <c r="AE28" s="92"/>
+      <c r="AA28" s="82"/>
+      <c r="AB28" s="82"/>
+      <c r="AC28" s="82"/>
+      <c r="AD28" s="82"/>
+      <c r="AE28" s="82"/>
       <c r="AF28" s="16"/>
       <c r="AG28" s="17"/>
-      <c r="AH28" s="93"/>
-      <c r="AI28" s="93"/>
+      <c r="AH28" s="83"/>
+      <c r="AI28" s="83"/>
     </row>
     <row r="29" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B29" s="95"/>
+      <c r="B29" s="80"/>
       <c r="C29" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="97">
+      <c r="E29" s="99">
         <f>C11</f>
         <v>0</v>
       </c>
-      <c r="F29" s="97"/>
+      <c r="F29" s="99"/>
       <c r="G29" s="25">
         <v>15</v>
       </c>
-      <c r="H29" s="86"/>
-      <c r="I29" s="86"/>
-      <c r="J29" s="86"/>
-      <c r="K29" s="86"/>
-      <c r="L29" s="86"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="92"/>
+      <c r="J29" s="92"/>
+      <c r="K29" s="92"/>
+      <c r="L29" s="92"/>
       <c r="M29" s="23"/>
       <c r="N29" s="24"/>
-      <c r="O29" s="93"/>
-      <c r="P29" s="93"/>
+      <c r="O29" s="83"/>
+      <c r="P29" s="83"/>
       <c r="Q29" s="53"/>
-      <c r="R29" s="107"/>
+      <c r="R29" s="95"/>
       <c r="S29" s="1"/>
-      <c r="T29" s="95"/>
+      <c r="T29" s="80"/>
       <c r="U29" s="20" t="s">
         <v>2</v>
       </c>
       <c r="V29" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="W29" s="94">
+      <c r="W29" s="91">
         <f>C10</f>
         <v>0</v>
       </c>
-      <c r="X29" s="94"/>
+      <c r="X29" s="91"/>
       <c r="Y29" s="22">
         <v>9</v>
       </c>
       <c r="Z29" s="25">
         <v>14</v>
       </c>
-      <c r="AA29" s="86"/>
-      <c r="AB29" s="86"/>
-      <c r="AC29" s="86"/>
-      <c r="AD29" s="86"/>
-      <c r="AE29" s="86"/>
+      <c r="AA29" s="92"/>
+      <c r="AB29" s="92"/>
+      <c r="AC29" s="92"/>
+      <c r="AD29" s="92"/>
+      <c r="AE29" s="92"/>
       <c r="AF29" s="23"/>
       <c r="AG29" s="24"/>
-      <c r="AH29" s="93"/>
-      <c r="AI29" s="93"/>
+      <c r="AH29" s="83"/>
+      <c r="AI29" s="83"/>
     </row>
     <row r="30" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B30" s="95"/>
+      <c r="B30" s="80"/>
       <c r="C30" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="94">
+      <c r="E30" s="91">
         <f>U11</f>
         <v>0</v>
       </c>
-      <c r="F30" s="94"/>
+      <c r="F30" s="91"/>
       <c r="G30" s="26">
         <v>7</v>
       </c>
-      <c r="H30" s="86"/>
-      <c r="I30" s="86"/>
-      <c r="J30" s="86"/>
-      <c r="K30" s="86"/>
-      <c r="L30" s="86"/>
+      <c r="H30" s="92"/>
+      <c r="I30" s="92"/>
+      <c r="J30" s="92"/>
+      <c r="K30" s="92"/>
+      <c r="L30" s="92"/>
       <c r="M30" s="23"/>
       <c r="N30" s="24"/>
-      <c r="O30" s="98"/>
-      <c r="P30" s="98"/>
+      <c r="O30" s="84"/>
+      <c r="P30" s="84"/>
       <c r="Q30" s="53"/>
-      <c r="R30" s="107"/>
+      <c r="R30" s="95"/>
       <c r="S30" s="1"/>
-      <c r="T30" s="95"/>
+      <c r="T30" s="80"/>
       <c r="U30" s="20" t="s">
         <v>14</v>
       </c>
       <c r="V30" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="W30" s="94">
+      <c r="W30" s="91">
         <f>U5</f>
         <v>0</v>
       </c>
-      <c r="X30" s="94"/>
+      <c r="X30" s="91"/>
       <c r="Y30" s="26">
         <v>2</v>
       </c>
       <c r="Z30" s="27">
         <v>1</v>
       </c>
-      <c r="AA30" s="86"/>
-      <c r="AB30" s="86"/>
-      <c r="AC30" s="86"/>
-      <c r="AD30" s="86"/>
-      <c r="AE30" s="86"/>
+      <c r="AA30" s="92"/>
+      <c r="AB30" s="92"/>
+      <c r="AC30" s="92"/>
+      <c r="AD30" s="92"/>
+      <c r="AE30" s="92"/>
       <c r="AF30" s="23"/>
       <c r="AG30" s="24"/>
-      <c r="AH30" s="98"/>
-      <c r="AI30" s="98"/>
+      <c r="AH30" s="84"/>
+      <c r="AI30" s="84"/>
     </row>
     <row r="31" spans="2:35" ht="13.5" customHeight="1">
       <c r="B31" s="28"/>
@@ -4286,25 +3965,25 @@
       <c r="D31" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="88">
+      <c r="E31" s="96">
         <f>C9</f>
         <v>0</v>
       </c>
-      <c r="F31" s="88"/>
+      <c r="F31" s="96"/>
       <c r="G31" s="34">
         <v>13</v>
       </c>
-      <c r="H31" s="89"/>
-      <c r="I31" s="89"/>
-      <c r="J31" s="89"/>
-      <c r="K31" s="89"/>
-      <c r="L31" s="89"/>
+      <c r="H31" s="97"/>
+      <c r="I31" s="97"/>
+      <c r="J31" s="97"/>
+      <c r="K31" s="97"/>
+      <c r="L31" s="97"/>
       <c r="M31" s="32"/>
       <c r="N31" s="33"/>
-      <c r="O31" s="98"/>
-      <c r="P31" s="98"/>
+      <c r="O31" s="84"/>
+      <c r="P31" s="84"/>
       <c r="Q31" s="53"/>
-      <c r="R31" s="107"/>
+      <c r="R31" s="95"/>
       <c r="S31" s="1"/>
       <c r="T31" s="28"/>
       <c r="U31" s="29" t="s">
@@ -4313,29 +3992,29 @@
       <c r="V31" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="W31" s="88">
+      <c r="W31" s="96">
         <f>C7</f>
         <v>0</v>
       </c>
-      <c r="X31" s="88"/>
+      <c r="X31" s="96"/>
       <c r="Y31" s="31">
         <v>10</v>
       </c>
       <c r="Z31" s="34">
         <v>11</v>
       </c>
-      <c r="AA31" s="89"/>
-      <c r="AB31" s="89"/>
-      <c r="AC31" s="89"/>
-      <c r="AD31" s="89"/>
-      <c r="AE31" s="89"/>
+      <c r="AA31" s="97"/>
+      <c r="AB31" s="97"/>
+      <c r="AC31" s="97"/>
+      <c r="AD31" s="97"/>
+      <c r="AE31" s="97"/>
       <c r="AF31" s="32"/>
       <c r="AG31" s="33"/>
-      <c r="AH31" s="98"/>
-      <c r="AI31" s="98"/>
+      <c r="AH31" s="84"/>
+      <c r="AI31" s="84"/>
     </row>
     <row r="32" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B32" s="95">
+      <c r="B32" s="80">
         <v>5</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -4344,27 +4023,27 @@
       <c r="D32" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="96">
+      <c r="E32" s="81">
         <f>C8</f>
         <v>0</v>
       </c>
-      <c r="F32" s="96"/>
+      <c r="F32" s="81"/>
       <c r="G32" s="35">
         <v>12</v>
       </c>
-      <c r="H32" s="92"/>
-      <c r="I32" s="92"/>
-      <c r="J32" s="92"/>
-      <c r="K32" s="92"/>
-      <c r="L32" s="92"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="82"/>
+      <c r="J32" s="82"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="82"/>
       <c r="M32" s="16"/>
       <c r="N32" s="17"/>
-      <c r="O32" s="93"/>
-      <c r="P32" s="93"/>
+      <c r="O32" s="83"/>
+      <c r="P32" s="83"/>
       <c r="Q32" s="53"/>
-      <c r="R32" s="107"/>
+      <c r="R32" s="95"/>
       <c r="S32" s="1"/>
-      <c r="T32" s="95">
+      <c r="T32" s="80">
         <v>13</v>
       </c>
       <c r="U32" s="13" t="s">
@@ -4373,138 +4052,138 @@
       <c r="V32" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W32" s="96">
+      <c r="W32" s="81">
         <f>C8</f>
         <v>0</v>
       </c>
-      <c r="X32" s="96"/>
+      <c r="X32" s="81"/>
       <c r="Y32" s="15">
         <v>1</v>
       </c>
       <c r="Z32" s="35">
         <v>12</v>
       </c>
-      <c r="AA32" s="92"/>
-      <c r="AB32" s="92"/>
-      <c r="AC32" s="92"/>
-      <c r="AD32" s="92"/>
-      <c r="AE32" s="92"/>
+      <c r="AA32" s="82"/>
+      <c r="AB32" s="82"/>
+      <c r="AC32" s="82"/>
+      <c r="AD32" s="82"/>
+      <c r="AE32" s="82"/>
       <c r="AF32" s="16"/>
       <c r="AG32" s="17"/>
-      <c r="AH32" s="93"/>
-      <c r="AI32" s="93"/>
+      <c r="AH32" s="83"/>
+      <c r="AI32" s="83"/>
     </row>
     <row r="33" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B33" s="95"/>
+      <c r="B33" s="80"/>
       <c r="C33" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="94">
+      <c r="E33" s="91">
         <f>U5</f>
         <v>0</v>
       </c>
-      <c r="F33" s="94"/>
+      <c r="F33" s="91"/>
       <c r="G33" s="27">
         <v>1</v>
       </c>
-      <c r="H33" s="86"/>
-      <c r="I33" s="86"/>
-      <c r="J33" s="86"/>
-      <c r="K33" s="86"/>
-      <c r="L33" s="86"/>
+      <c r="H33" s="92"/>
+      <c r="I33" s="92"/>
+      <c r="J33" s="92"/>
+      <c r="K33" s="92"/>
+      <c r="L33" s="92"/>
       <c r="M33" s="23"/>
       <c r="N33" s="24"/>
-      <c r="O33" s="93"/>
-      <c r="P33" s="93"/>
+      <c r="O33" s="83"/>
+      <c r="P33" s="83"/>
       <c r="Q33" s="53"/>
-      <c r="R33" s="107"/>
+      <c r="R33" s="95"/>
       <c r="S33" s="1"/>
-      <c r="T33" s="95"/>
+      <c r="T33" s="80"/>
       <c r="U33" s="20" t="s">
         <v>2</v>
       </c>
       <c r="V33" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="W33" s="94">
+      <c r="W33" s="91">
         <f>U8</f>
         <v>0</v>
       </c>
-      <c r="X33" s="94"/>
+      <c r="X33" s="91"/>
       <c r="Y33" s="22">
         <v>9</v>
       </c>
       <c r="Z33" s="39">
         <v>4</v>
       </c>
-      <c r="AA33" s="86"/>
-      <c r="AB33" s="86"/>
-      <c r="AC33" s="86"/>
-      <c r="AD33" s="86"/>
-      <c r="AE33" s="86"/>
+      <c r="AA33" s="92"/>
+      <c r="AB33" s="92"/>
+      <c r="AC33" s="92"/>
+      <c r="AD33" s="92"/>
+      <c r="AE33" s="92"/>
       <c r="AF33" s="23"/>
       <c r="AG33" s="24"/>
-      <c r="AH33" s="93"/>
-      <c r="AI33" s="93"/>
+      <c r="AH33" s="83"/>
+      <c r="AI33" s="83"/>
     </row>
     <row r="34" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B34" s="95"/>
+      <c r="B34" s="80"/>
       <c r="C34" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="94">
+      <c r="E34" s="91">
         <f>C7</f>
         <v>0</v>
       </c>
-      <c r="F34" s="94"/>
+      <c r="F34" s="91"/>
       <c r="G34" s="22">
         <v>11</v>
       </c>
-      <c r="H34" s="86"/>
-      <c r="I34" s="86"/>
-      <c r="J34" s="86"/>
-      <c r="K34" s="86"/>
-      <c r="L34" s="86"/>
+      <c r="H34" s="92"/>
+      <c r="I34" s="92"/>
+      <c r="J34" s="92"/>
+      <c r="K34" s="92"/>
+      <c r="L34" s="92"/>
       <c r="M34" s="23"/>
       <c r="N34" s="24"/>
       <c r="O34" s="100"/>
       <c r="P34" s="100"/>
       <c r="Q34" s="53"/>
-      <c r="R34" s="107"/>
+      <c r="R34" s="95"/>
       <c r="S34" s="1"/>
-      <c r="T34" s="95"/>
+      <c r="T34" s="80"/>
       <c r="U34" s="20" t="s">
         <v>14</v>
       </c>
       <c r="V34" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="W34" s="94">
+      <c r="W34" s="91">
         <f>C5</f>
         <v>0</v>
       </c>
-      <c r="X34" s="94"/>
+      <c r="X34" s="91"/>
       <c r="Y34" s="26">
         <v>2</v>
       </c>
       <c r="Z34" s="22">
         <v>9</v>
       </c>
-      <c r="AA34" s="86"/>
-      <c r="AB34" s="86"/>
-      <c r="AC34" s="86"/>
-      <c r="AD34" s="86"/>
-      <c r="AE34" s="86"/>
+      <c r="AA34" s="92"/>
+      <c r="AB34" s="92"/>
+      <c r="AC34" s="92"/>
+      <c r="AD34" s="92"/>
+      <c r="AE34" s="92"/>
       <c r="AF34" s="23"/>
       <c r="AG34" s="24"/>
-      <c r="AH34" s="98"/>
-      <c r="AI34" s="98"/>
+      <c r="AH34" s="84"/>
+      <c r="AI34" s="84"/>
     </row>
     <row r="35" spans="2:35" ht="13.5" customHeight="1">
       <c r="B35" s="28"/>
@@ -4514,25 +4193,25 @@
       <c r="D35" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="88">
+      <c r="E35" s="96">
         <f>U6</f>
         <v>0</v>
       </c>
-      <c r="F35" s="88"/>
+      <c r="F35" s="96"/>
       <c r="G35" s="41">
         <v>2</v>
       </c>
-      <c r="H35" s="89"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="89"/>
-      <c r="K35" s="89"/>
-      <c r="L35" s="89"/>
+      <c r="H35" s="97"/>
+      <c r="I35" s="97"/>
+      <c r="J35" s="97"/>
+      <c r="K35" s="97"/>
+      <c r="L35" s="97"/>
       <c r="M35" s="32"/>
       <c r="N35" s="33"/>
       <c r="O35" s="100"/>
       <c r="P35" s="100"/>
       <c r="Q35" s="53"/>
-      <c r="R35" s="107"/>
+      <c r="R35" s="95"/>
       <c r="S35" s="1"/>
       <c r="T35" s="42"/>
       <c r="U35" s="29" t="s">
@@ -4541,29 +4220,29 @@
       <c r="V35" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="W35" s="88">
+      <c r="W35" s="96">
         <f>U9</f>
         <v>0</v>
       </c>
-      <c r="X35" s="88"/>
+      <c r="X35" s="96"/>
       <c r="Y35" s="31">
         <v>10</v>
       </c>
       <c r="Z35" s="40">
         <v>5</v>
       </c>
-      <c r="AA35" s="89"/>
-      <c r="AB35" s="89"/>
-      <c r="AC35" s="89"/>
-      <c r="AD35" s="89"/>
-      <c r="AE35" s="89"/>
+      <c r="AA35" s="97"/>
+      <c r="AB35" s="97"/>
+      <c r="AC35" s="97"/>
+      <c r="AD35" s="97"/>
+      <c r="AE35" s="97"/>
       <c r="AF35" s="32"/>
       <c r="AG35" s="33"/>
-      <c r="AH35" s="98"/>
-      <c r="AI35" s="98"/>
+      <c r="AH35" s="84"/>
+      <c r="AI35" s="84"/>
     </row>
     <row r="36" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B36" s="95">
+      <c r="B36" s="80">
         <v>6</v>
       </c>
       <c r="C36" s="13" t="s">
@@ -4572,25 +4251,25 @@
       <c r="D36" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E36" s="96">
+      <c r="E36" s="81">
         <f>U7</f>
         <v>0</v>
       </c>
-      <c r="F36" s="96"/>
+      <c r="F36" s="81"/>
       <c r="G36" s="15">
         <v>3</v>
       </c>
-      <c r="H36" s="92"/>
-      <c r="I36" s="92"/>
-      <c r="J36" s="92"/>
-      <c r="K36" s="92"/>
-      <c r="L36" s="92"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="82"/>
       <c r="M36" s="16"/>
       <c r="N36" s="17"/>
-      <c r="O36" s="93"/>
-      <c r="P36" s="93"/>
+      <c r="O36" s="83"/>
+      <c r="P36" s="83"/>
       <c r="Q36" s="53"/>
-      <c r="R36" s="107"/>
+      <c r="R36" s="95"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
@@ -4610,94 +4289,94 @@
       <c r="AI36" s="1"/>
     </row>
     <row r="37" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B37" s="95"/>
+      <c r="B37" s="80"/>
       <c r="C37" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="94">
+      <c r="E37" s="91">
         <f>C9</f>
         <v>0</v>
       </c>
-      <c r="F37" s="94"/>
+      <c r="F37" s="91"/>
       <c r="G37" s="22">
         <v>13</v>
       </c>
-      <c r="H37" s="86"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="86"/>
-      <c r="K37" s="86"/>
-      <c r="L37" s="86"/>
+      <c r="H37" s="92"/>
+      <c r="I37" s="92"/>
+      <c r="J37" s="92"/>
+      <c r="K37" s="92"/>
+      <c r="L37" s="92"/>
       <c r="M37" s="23"/>
       <c r="N37" s="24"/>
-      <c r="O37" s="93"/>
-      <c r="P37" s="93"/>
+      <c r="O37" s="83"/>
+      <c r="P37" s="83"/>
       <c r="Q37" s="53"/>
-      <c r="R37" s="107"/>
+      <c r="R37" s="95"/>
       <c r="S37" s="1"/>
-      <c r="T37" s="99"/>
-      <c r="U37" s="99"/>
-      <c r="V37" s="99"/>
-      <c r="W37" s="99"/>
-      <c r="X37" s="99"/>
-      <c r="Y37" s="99"/>
-      <c r="Z37" s="99"/>
-      <c r="AA37" s="99"/>
-      <c r="AB37" s="99"/>
-      <c r="AC37" s="99"/>
-      <c r="AD37" s="99"/>
-      <c r="AE37" s="99"/>
-      <c r="AF37" s="99"/>
-      <c r="AG37" s="99"/>
-      <c r="AH37" s="99"/>
-      <c r="AI37" s="99"/>
+      <c r="T37" s="101"/>
+      <c r="U37" s="101"/>
+      <c r="V37" s="101"/>
+      <c r="W37" s="101"/>
+      <c r="X37" s="101"/>
+      <c r="Y37" s="101"/>
+      <c r="Z37" s="101"/>
+      <c r="AA37" s="101"/>
+      <c r="AB37" s="101"/>
+      <c r="AC37" s="101"/>
+      <c r="AD37" s="101"/>
+      <c r="AE37" s="101"/>
+      <c r="AF37" s="101"/>
+      <c r="AG37" s="101"/>
+      <c r="AH37" s="101"/>
+      <c r="AI37" s="101"/>
     </row>
     <row r="38" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B38" s="95"/>
+      <c r="B38" s="80"/>
       <c r="C38" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="94">
+      <c r="E38" s="91">
         <f>U8</f>
         <v>0</v>
       </c>
-      <c r="F38" s="94"/>
+      <c r="F38" s="91"/>
       <c r="G38" s="26">
         <v>4</v>
       </c>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="86"/>
-      <c r="L38" s="86"/>
+      <c r="H38" s="92"/>
+      <c r="I38" s="92"/>
+      <c r="J38" s="92"/>
+      <c r="K38" s="92"/>
+      <c r="L38" s="92"/>
       <c r="M38" s="23"/>
       <c r="N38" s="24"/>
-      <c r="O38" s="98"/>
-      <c r="P38" s="98"/>
+      <c r="O38" s="84"/>
+      <c r="P38" s="84"/>
       <c r="Q38" s="53"/>
-      <c r="R38" s="107"/>
+      <c r="R38" s="95"/>
       <c r="S38" s="1"/>
-      <c r="T38" s="99"/>
-      <c r="U38" s="99"/>
-      <c r="V38" s="99"/>
-      <c r="W38" s="99"/>
-      <c r="X38" s="99"/>
-      <c r="Y38" s="99"/>
-      <c r="Z38" s="99"/>
-      <c r="AA38" s="99"/>
-      <c r="AB38" s="99"/>
-      <c r="AC38" s="99"/>
-      <c r="AD38" s="99"/>
-      <c r="AE38" s="99"/>
-      <c r="AF38" s="99"/>
-      <c r="AG38" s="99"/>
-      <c r="AH38" s="99"/>
-      <c r="AI38" s="99"/>
+      <c r="T38" s="101"/>
+      <c r="U38" s="101"/>
+      <c r="V38" s="101"/>
+      <c r="W38" s="101"/>
+      <c r="X38" s="101"/>
+      <c r="Y38" s="101"/>
+      <c r="Z38" s="101"/>
+      <c r="AA38" s="101"/>
+      <c r="AB38" s="101"/>
+      <c r="AC38" s="101"/>
+      <c r="AD38" s="101"/>
+      <c r="AE38" s="101"/>
+      <c r="AF38" s="101"/>
+      <c r="AG38" s="101"/>
+      <c r="AH38" s="101"/>
+      <c r="AI38" s="101"/>
     </row>
     <row r="39" spans="2:35" ht="13.5" customHeight="1">
       <c r="B39" s="28"/>
@@ -4707,25 +4386,25 @@
       <c r="D39" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E39" s="88">
+      <c r="E39" s="96">
         <f>C10</f>
         <v>0</v>
       </c>
-      <c r="F39" s="88"/>
+      <c r="F39" s="96"/>
       <c r="G39" s="43">
         <v>14</v>
       </c>
-      <c r="H39" s="89"/>
-      <c r="I39" s="89"/>
-      <c r="J39" s="89"/>
-      <c r="K39" s="89"/>
-      <c r="L39" s="89"/>
+      <c r="H39" s="97"/>
+      <c r="I39" s="97"/>
+      <c r="J39" s="97"/>
+      <c r="K39" s="97"/>
+      <c r="L39" s="97"/>
       <c r="M39" s="32"/>
       <c r="N39" s="33"/>
-      <c r="O39" s="98"/>
-      <c r="P39" s="98"/>
+      <c r="O39" s="84"/>
+      <c r="P39" s="84"/>
       <c r="Q39" s="53"/>
-      <c r="R39" s="107"/>
+      <c r="R39" s="95"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
@@ -4745,7 +4424,7 @@
       <c r="AI39" s="1"/>
     </row>
     <row r="40" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B40" s="95">
+      <c r="B40" s="80">
         <v>7</v>
       </c>
       <c r="C40" s="13" t="s">
@@ -4754,27 +4433,27 @@
       <c r="D40" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="96">
+      <c r="E40" s="81">
         <f>C5</f>
         <v>0</v>
       </c>
-      <c r="F40" s="96"/>
+      <c r="F40" s="81"/>
       <c r="G40" s="38">
         <v>9</v>
       </c>
-      <c r="H40" s="92"/>
-      <c r="I40" s="92"/>
-      <c r="J40" s="92"/>
-      <c r="K40" s="92"/>
-      <c r="L40" s="92"/>
+      <c r="H40" s="82"/>
+      <c r="I40" s="82"/>
+      <c r="J40" s="82"/>
+      <c r="K40" s="82"/>
+      <c r="L40" s="82"/>
       <c r="M40" s="16"/>
       <c r="N40" s="17"/>
-      <c r="O40" s="93"/>
-      <c r="P40" s="93"/>
+      <c r="O40" s="83"/>
+      <c r="P40" s="83"/>
       <c r="Q40" s="53"/>
-      <c r="R40" s="107"/>
+      <c r="R40" s="95"/>
       <c r="S40" s="1"/>
-      <c r="T40" s="95">
+      <c r="T40" s="80">
         <v>14</v>
       </c>
       <c r="U40" s="44" t="s">
@@ -4783,123 +4462,123 @@
       <c r="V40" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="W40" s="91"/>
-      <c r="X40" s="91"/>
+      <c r="W40" s="103"/>
+      <c r="X40" s="103"/>
       <c r="Y40" s="46">
         <v>1</v>
       </c>
       <c r="Z40" s="46"/>
-      <c r="AA40" s="92"/>
-      <c r="AB40" s="92"/>
-      <c r="AC40" s="92"/>
-      <c r="AD40" s="92"/>
-      <c r="AE40" s="92"/>
+      <c r="AA40" s="82"/>
+      <c r="AB40" s="82"/>
+      <c r="AC40" s="82"/>
+      <c r="AD40" s="82"/>
+      <c r="AE40" s="82"/>
       <c r="AF40" s="47"/>
       <c r="AG40" s="48"/>
-      <c r="AH40" s="93"/>
-      <c r="AI40" s="93"/>
+      <c r="AH40" s="83"/>
+      <c r="AI40" s="83"/>
     </row>
     <row r="41" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B41" s="95"/>
+      <c r="B41" s="80"/>
       <c r="C41" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E41" s="94">
+      <c r="E41" s="91">
         <f>U9</f>
         <v>0</v>
       </c>
-      <c r="F41" s="94"/>
+      <c r="F41" s="91"/>
       <c r="G41" s="27">
         <v>5</v>
       </c>
-      <c r="H41" s="86"/>
-      <c r="I41" s="86"/>
-      <c r="J41" s="86"/>
-      <c r="K41" s="86"/>
-      <c r="L41" s="86"/>
+      <c r="H41" s="92"/>
+      <c r="I41" s="92"/>
+      <c r="J41" s="92"/>
+      <c r="K41" s="92"/>
+      <c r="L41" s="92"/>
       <c r="M41" s="23"/>
       <c r="N41" s="24"/>
-      <c r="O41" s="93"/>
-      <c r="P41" s="93"/>
+      <c r="O41" s="83"/>
+      <c r="P41" s="83"/>
       <c r="Q41" s="53"/>
-      <c r="R41" s="107"/>
+      <c r="R41" s="95"/>
       <c r="S41" s="1"/>
-      <c r="T41" s="95"/>
+      <c r="T41" s="80"/>
       <c r="U41" s="20" t="s">
         <v>2</v>
       </c>
       <c r="V41" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="W41" s="85"/>
-      <c r="X41" s="85"/>
+      <c r="W41" s="104"/>
+      <c r="X41" s="104"/>
       <c r="Y41" s="22">
         <v>9</v>
       </c>
       <c r="Z41" s="22"/>
-      <c r="AA41" s="86"/>
-      <c r="AB41" s="86"/>
-      <c r="AC41" s="86"/>
-      <c r="AD41" s="86"/>
-      <c r="AE41" s="86"/>
+      <c r="AA41" s="92"/>
+      <c r="AB41" s="92"/>
+      <c r="AC41" s="92"/>
+      <c r="AD41" s="92"/>
+      <c r="AE41" s="92"/>
       <c r="AF41" s="23"/>
       <c r="AG41" s="24"/>
-      <c r="AH41" s="93"/>
-      <c r="AI41" s="93"/>
+      <c r="AH41" s="83"/>
+      <c r="AI41" s="83"/>
     </row>
     <row r="42" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B42" s="95"/>
+      <c r="B42" s="80"/>
       <c r="C42" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="94">
+      <c r="E42" s="91">
         <f>C6</f>
         <v>0</v>
       </c>
-      <c r="F42" s="94"/>
+      <c r="F42" s="91"/>
       <c r="G42" s="25">
         <v>10</v>
       </c>
-      <c r="H42" s="86"/>
-      <c r="I42" s="86"/>
-      <c r="J42" s="86"/>
-      <c r="K42" s="86"/>
-      <c r="L42" s="86"/>
+      <c r="H42" s="92"/>
+      <c r="I42" s="92"/>
+      <c r="J42" s="92"/>
+      <c r="K42" s="92"/>
+      <c r="L42" s="92"/>
       <c r="M42" s="23"/>
       <c r="N42" s="24"/>
-      <c r="O42" s="98"/>
-      <c r="P42" s="98"/>
+      <c r="O42" s="84"/>
+      <c r="P42" s="84"/>
       <c r="Q42" s="53"/>
-      <c r="R42" s="107"/>
+      <c r="R42" s="95"/>
       <c r="S42" s="1"/>
-      <c r="T42" s="95"/>
+      <c r="T42" s="80"/>
       <c r="U42" s="20" t="s">
         <v>14</v>
       </c>
       <c r="V42" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="W42" s="85"/>
-      <c r="X42" s="85"/>
+      <c r="W42" s="104"/>
+      <c r="X42" s="104"/>
       <c r="Y42" s="26">
         <v>2</v>
       </c>
       <c r="Z42" s="39"/>
-      <c r="AA42" s="86"/>
-      <c r="AB42" s="86"/>
-      <c r="AC42" s="86"/>
-      <c r="AD42" s="86"/>
-      <c r="AE42" s="86"/>
+      <c r="AA42" s="92"/>
+      <c r="AB42" s="92"/>
+      <c r="AC42" s="92"/>
+      <c r="AD42" s="92"/>
+      <c r="AE42" s="92"/>
       <c r="AF42" s="23"/>
       <c r="AG42" s="24"/>
-      <c r="AH42" s="98"/>
-      <c r="AI42" s="98"/>
+      <c r="AH42" s="84"/>
+      <c r="AI42" s="84"/>
     </row>
     <row r="43" spans="2:35" ht="13.5" customHeight="1">
       <c r="B43" s="28"/>
@@ -4909,25 +4588,25 @@
       <c r="D43" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E43" s="88">
+      <c r="E43" s="96">
         <f>U10</f>
         <v>0</v>
       </c>
-      <c r="F43" s="88"/>
+      <c r="F43" s="96"/>
       <c r="G43" s="41">
         <v>6</v>
       </c>
-      <c r="H43" s="89"/>
-      <c r="I43" s="89"/>
-      <c r="J43" s="89"/>
-      <c r="K43" s="89"/>
-      <c r="L43" s="89"/>
+      <c r="H43" s="97"/>
+      <c r="I43" s="97"/>
+      <c r="J43" s="97"/>
+      <c r="K43" s="97"/>
+      <c r="L43" s="97"/>
       <c r="M43" s="32"/>
       <c r="N43" s="33"/>
-      <c r="O43" s="98"/>
-      <c r="P43" s="98"/>
+      <c r="O43" s="84"/>
+      <c r="P43" s="84"/>
       <c r="Q43" s="53"/>
-      <c r="R43" s="107"/>
+      <c r="R43" s="95"/>
       <c r="S43" s="1"/>
       <c r="T43" s="28"/>
       <c r="U43" s="29" t="s">
@@ -4936,24 +4615,24 @@
       <c r="V43" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="W43" s="90"/>
-      <c r="X43" s="90"/>
+      <c r="W43" s="102"/>
+      <c r="X43" s="102"/>
       <c r="Y43" s="31">
         <v>10</v>
       </c>
       <c r="Z43" s="31"/>
-      <c r="AA43" s="89"/>
-      <c r="AB43" s="89"/>
-      <c r="AC43" s="89"/>
-      <c r="AD43" s="89"/>
-      <c r="AE43" s="89"/>
+      <c r="AA43" s="97"/>
+      <c r="AB43" s="97"/>
+      <c r="AC43" s="97"/>
+      <c r="AD43" s="97"/>
+      <c r="AE43" s="97"/>
       <c r="AF43" s="32"/>
       <c r="AG43" s="33"/>
-      <c r="AH43" s="98"/>
-      <c r="AI43" s="98"/>
+      <c r="AH43" s="84"/>
+      <c r="AI43" s="84"/>
     </row>
     <row r="44" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B44" s="95">
+      <c r="B44" s="80">
         <v>8</v>
       </c>
       <c r="C44" s="13" t="s">
@@ -4962,27 +4641,27 @@
       <c r="D44" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="96">
+      <c r="E44" s="81">
         <f>C9</f>
         <v>0</v>
       </c>
-      <c r="F44" s="96"/>
+      <c r="F44" s="81"/>
       <c r="G44" s="38">
         <v>13</v>
       </c>
-      <c r="H44" s="92"/>
-      <c r="I44" s="92"/>
-      <c r="J44" s="92"/>
-      <c r="K44" s="92"/>
-      <c r="L44" s="92"/>
+      <c r="H44" s="82"/>
+      <c r="I44" s="82"/>
+      <c r="J44" s="82"/>
+      <c r="K44" s="82"/>
+      <c r="L44" s="82"/>
       <c r="M44" s="16"/>
       <c r="N44" s="17"/>
-      <c r="O44" s="93"/>
-      <c r="P44" s="93"/>
+      <c r="O44" s="83"/>
+      <c r="P44" s="83"/>
       <c r="Q44" s="53"/>
-      <c r="R44" s="107"/>
+      <c r="R44" s="95"/>
       <c r="S44" s="1"/>
-      <c r="T44" s="95">
+      <c r="T44" s="80">
         <v>15</v>
       </c>
       <c r="U44" s="13" t="s">
@@ -4991,123 +4670,123 @@
       <c r="V44" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W44" s="91"/>
-      <c r="X44" s="91"/>
+      <c r="W44" s="103"/>
+      <c r="X44" s="103"/>
       <c r="Y44" s="15">
         <v>1</v>
       </c>
       <c r="Z44" s="38"/>
-      <c r="AA44" s="92"/>
-      <c r="AB44" s="92"/>
-      <c r="AC44" s="92"/>
-      <c r="AD44" s="92"/>
-      <c r="AE44" s="92"/>
+      <c r="AA44" s="82"/>
+      <c r="AB44" s="82"/>
+      <c r="AC44" s="82"/>
+      <c r="AD44" s="82"/>
+      <c r="AE44" s="82"/>
       <c r="AF44" s="16"/>
       <c r="AG44" s="17"/>
-      <c r="AH44" s="93"/>
-      <c r="AI44" s="93"/>
+      <c r="AH44" s="83"/>
+      <c r="AI44" s="83"/>
     </row>
     <row r="45" spans="2:35" ht="13.5" customHeight="1">
-      <c r="B45" s="95"/>
+      <c r="B45" s="80"/>
       <c r="C45" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D45" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E45" s="94">
+      <c r="E45" s="91">
         <f>U6</f>
         <v>0</v>
       </c>
-      <c r="F45" s="94"/>
+      <c r="F45" s="91"/>
       <c r="G45" s="39">
         <v>2</v>
       </c>
-      <c r="H45" s="86"/>
-      <c r="I45" s="86"/>
-      <c r="J45" s="86"/>
-      <c r="K45" s="86"/>
-      <c r="L45" s="86"/>
+      <c r="H45" s="92"/>
+      <c r="I45" s="92"/>
+      <c r="J45" s="92"/>
+      <c r="K45" s="92"/>
+      <c r="L45" s="92"/>
       <c r="M45" s="23"/>
       <c r="N45" s="24"/>
-      <c r="O45" s="93"/>
-      <c r="P45" s="93"/>
+      <c r="O45" s="83"/>
+      <c r="P45" s="83"/>
       <c r="Q45" s="53"/>
-      <c r="R45" s="107"/>
+      <c r="R45" s="95"/>
       <c r="S45" s="1"/>
-      <c r="T45" s="95"/>
+      <c r="T45" s="80"/>
       <c r="U45" s="20" t="s">
         <v>2</v>
       </c>
       <c r="V45" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="W45" s="85"/>
-      <c r="X45" s="85"/>
+      <c r="W45" s="104"/>
+      <c r="X45" s="104"/>
       <c r="Y45" s="22">
         <v>9</v>
       </c>
       <c r="Z45" s="27"/>
-      <c r="AA45" s="86"/>
-      <c r="AB45" s="86"/>
-      <c r="AC45" s="86"/>
-      <c r="AD45" s="86"/>
-      <c r="AE45" s="86"/>
+      <c r="AA45" s="92"/>
+      <c r="AB45" s="92"/>
+      <c r="AC45" s="92"/>
+      <c r="AD45" s="92"/>
+      <c r="AE45" s="92"/>
       <c r="AF45" s="23"/>
       <c r="AG45" s="24"/>
-      <c r="AH45" s="93"/>
-      <c r="AI45" s="93"/>
+      <c r="AH45" s="83"/>
+      <c r="AI45" s="83"/>
     </row>
     <row r="46" spans="2:35" ht="12.75" customHeight="1">
-      <c r="B46" s="95"/>
+      <c r="B46" s="80"/>
       <c r="C46" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="97">
+      <c r="E46" s="99">
         <f>C11</f>
         <v>0</v>
       </c>
-      <c r="F46" s="97"/>
+      <c r="F46" s="99"/>
       <c r="G46" s="25">
         <v>15</v>
       </c>
-      <c r="H46" s="86"/>
-      <c r="I46" s="86"/>
-      <c r="J46" s="86"/>
-      <c r="K46" s="86"/>
-      <c r="L46" s="86"/>
+      <c r="H46" s="92"/>
+      <c r="I46" s="92"/>
+      <c r="J46" s="92"/>
+      <c r="K46" s="92"/>
+      <c r="L46" s="92"/>
       <c r="M46" s="23"/>
       <c r="N46" s="24"/>
-      <c r="O46" s="98"/>
-      <c r="P46" s="98"/>
+      <c r="O46" s="84"/>
+      <c r="P46" s="84"/>
       <c r="Q46" s="53"/>
-      <c r="R46" s="107"/>
+      <c r="R46" s="95"/>
       <c r="S46" s="1"/>
-      <c r="T46" s="95"/>
+      <c r="T46" s="80"/>
       <c r="U46" s="20" t="s">
         <v>14</v>
       </c>
       <c r="V46" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="W46" s="85"/>
-      <c r="X46" s="85"/>
+      <c r="W46" s="104"/>
+      <c r="X46" s="104"/>
       <c r="Y46" s="26">
         <v>2</v>
       </c>
       <c r="Z46" s="25"/>
-      <c r="AA46" s="86"/>
-      <c r="AB46" s="86"/>
-      <c r="AC46" s="86"/>
-      <c r="AD46" s="86"/>
-      <c r="AE46" s="86"/>
+      <c r="AA46" s="92"/>
+      <c r="AB46" s="92"/>
+      <c r="AC46" s="92"/>
+      <c r="AD46" s="92"/>
+      <c r="AE46" s="92"/>
       <c r="AF46" s="23"/>
       <c r="AG46" s="24"/>
-      <c r="AH46" s="87"/>
-      <c r="AI46" s="87"/>
+      <c r="AH46" s="116"/>
+      <c r="AI46" s="116"/>
     </row>
     <row r="47" spans="2:35" ht="13.5" customHeight="1">
       <c r="B47" s="42"/>
@@ -5117,25 +4796,25 @@
       <c r="D47" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E47" s="88">
+      <c r="E47" s="96">
         <f>U5</f>
         <v>0</v>
       </c>
-      <c r="F47" s="88"/>
+      <c r="F47" s="96"/>
       <c r="G47" s="40">
         <v>1</v>
       </c>
-      <c r="H47" s="89"/>
-      <c r="I47" s="89"/>
-      <c r="J47" s="89"/>
-      <c r="K47" s="89"/>
-      <c r="L47" s="89"/>
+      <c r="H47" s="97"/>
+      <c r="I47" s="97"/>
+      <c r="J47" s="97"/>
+      <c r="K47" s="97"/>
+      <c r="L47" s="97"/>
       <c r="M47" s="32"/>
       <c r="N47" s="33"/>
-      <c r="O47" s="98"/>
-      <c r="P47" s="98"/>
+      <c r="O47" s="84"/>
+      <c r="P47" s="84"/>
       <c r="Q47" s="53"/>
-      <c r="R47" s="107"/>
+      <c r="R47" s="95"/>
       <c r="S47" s="1"/>
       <c r="T47" s="28"/>
       <c r="U47" s="29" t="s">
@@ -5144,21 +4823,21 @@
       <c r="V47" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="W47" s="90"/>
-      <c r="X47" s="90"/>
+      <c r="W47" s="102"/>
+      <c r="X47" s="102"/>
       <c r="Y47" s="31">
         <v>10</v>
       </c>
       <c r="Z47" s="41"/>
-      <c r="AA47" s="89"/>
-      <c r="AB47" s="89"/>
-      <c r="AC47" s="89"/>
-      <c r="AD47" s="89"/>
-      <c r="AE47" s="89"/>
+      <c r="AA47" s="97"/>
+      <c r="AB47" s="97"/>
+      <c r="AC47" s="97"/>
+      <c r="AD47" s="97"/>
+      <c r="AE47" s="97"/>
       <c r="AF47" s="32"/>
       <c r="AG47" s="33"/>
-      <c r="AH47" s="87"/>
-      <c r="AI47" s="87"/>
+      <c r="AH47" s="116"/>
+      <c r="AI47" s="116"/>
     </row>
     <row r="48" spans="2:35" ht="14.25" customHeight="1">
       <c r="B48" s="1"/>
@@ -5197,50 +4876,200 @@
       <c r="AI48" s="1"/>
     </row>
     <row r="49" spans="2:6">
-      <c r="B49" s="78"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="78"/>
-      <c r="E49" s="78"/>
-      <c r="F49" s="78"/>
+      <c r="B49" s="109"/>
+      <c r="C49" s="109"/>
+      <c r="D49" s="109"/>
+      <c r="E49" s="109"/>
+      <c r="F49" s="109"/>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="78"/>
-      <c r="C50" s="78"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="78"/>
-      <c r="F50" s="78"/>
+      <c r="B50" s="109"/>
+      <c r="C50" s="109"/>
+      <c r="D50" s="109"/>
+      <c r="E50" s="109"/>
+      <c r="F50" s="109"/>
     </row>
     <row r="51" spans="2:6" ht="14.25" customHeight="1"/>
     <row r="52" spans="2:6" ht="14.25" customHeight="1"/>
     <row r="53" spans="2:6" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="226">
-    <mergeCell ref="U5:X5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="U6:X6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="U7:X7"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="U12:X12"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="U8:X8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="U9:X9"/>
-    <mergeCell ref="U10:X10"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="T16:T18"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="C2:O3"/>
-    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="U2:AH3"/>
+    <mergeCell ref="B49:F50"/>
+    <mergeCell ref="B13:N13"/>
+    <mergeCell ref="T13:AG13"/>
+    <mergeCell ref="W46:X46"/>
+    <mergeCell ref="AA46:AE46"/>
+    <mergeCell ref="AH46:AH47"/>
+    <mergeCell ref="AI46:AI47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="H47:L47"/>
+    <mergeCell ref="W47:X47"/>
+    <mergeCell ref="AA47:AE47"/>
+    <mergeCell ref="W44:X44"/>
+    <mergeCell ref="AA44:AE44"/>
+    <mergeCell ref="AH44:AH45"/>
+    <mergeCell ref="AI44:AI45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="H45:L45"/>
+    <mergeCell ref="W45:X45"/>
+    <mergeCell ref="AA45:AE45"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="H44:L44"/>
+    <mergeCell ref="O44:O45"/>
+    <mergeCell ref="P44:P45"/>
+    <mergeCell ref="T44:T46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="H46:L46"/>
+    <mergeCell ref="O46:O47"/>
+    <mergeCell ref="P46:P47"/>
+    <mergeCell ref="W42:X42"/>
+    <mergeCell ref="AA42:AE42"/>
+    <mergeCell ref="AH42:AH43"/>
+    <mergeCell ref="AI42:AI43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="W43:X43"/>
+    <mergeCell ref="AA43:AE43"/>
+    <mergeCell ref="W40:X40"/>
+    <mergeCell ref="AA40:AE40"/>
+    <mergeCell ref="AH40:AH41"/>
+    <mergeCell ref="AI40:AI41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="W41:X41"/>
+    <mergeCell ref="AA41:AE41"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="O40:O41"/>
+    <mergeCell ref="P40:P41"/>
+    <mergeCell ref="T40:T42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="P42:P43"/>
+    <mergeCell ref="T37:AI38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="P38:P39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="O36:O37"/>
+    <mergeCell ref="P36:P37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="W34:X34"/>
+    <mergeCell ref="AA34:AE34"/>
+    <mergeCell ref="AH34:AH35"/>
+    <mergeCell ref="AI34:AI35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="W35:X35"/>
+    <mergeCell ref="AA35:AE35"/>
+    <mergeCell ref="W32:X32"/>
+    <mergeCell ref="AA32:AE32"/>
+    <mergeCell ref="AH32:AH33"/>
+    <mergeCell ref="AI32:AI33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="H33:L33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="AA33:AE33"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="P32:P33"/>
+    <mergeCell ref="T32:T34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="H34:L34"/>
+    <mergeCell ref="O34:O35"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="W30:X30"/>
+    <mergeCell ref="AA30:AE30"/>
+    <mergeCell ref="AH30:AH31"/>
+    <mergeCell ref="AI30:AI31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="W31:X31"/>
+    <mergeCell ref="AA31:AE31"/>
+    <mergeCell ref="W28:X28"/>
+    <mergeCell ref="AA28:AE28"/>
+    <mergeCell ref="AH28:AH29"/>
+    <mergeCell ref="AI28:AI29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="W29:X29"/>
+    <mergeCell ref="AA29:AE29"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="T28:T30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="AA26:AE26"/>
+    <mergeCell ref="AH26:AH27"/>
+    <mergeCell ref="AI26:AI27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="AA27:AE27"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="AA24:AE24"/>
+    <mergeCell ref="AH24:AH25"/>
+    <mergeCell ref="AI24:AI25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="H25:L25"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="AA25:AE25"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="H24:L24"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="T24:T26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="AH22:AH23"/>
+    <mergeCell ref="AI22:AI23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="H23:L23"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="AA23:AE23"/>
+    <mergeCell ref="W20:X20"/>
+    <mergeCell ref="AA20:AE20"/>
+    <mergeCell ref="AH20:AH21"/>
+    <mergeCell ref="AI20:AI21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="AA21:AE21"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="AA18:AE18"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="T20:T22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="AA22:AE22"/>
     <mergeCell ref="W16:X16"/>
     <mergeCell ref="AA16:AE16"/>
     <mergeCell ref="U11:X11"/>
@@ -5265,182 +5094,32 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="H18:L18"/>
     <mergeCell ref="O18:O19"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="AA18:AE18"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="T20:T22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="H22:L22"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="AA22:AE22"/>
-    <mergeCell ref="AH22:AH23"/>
-    <mergeCell ref="AI22:AI23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="H23:L23"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="AA23:AE23"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="AA20:AE20"/>
-    <mergeCell ref="AH20:AH21"/>
-    <mergeCell ref="AI20:AI21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="AA21:AE21"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="H24:L24"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="T24:T26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="AA26:AE26"/>
-    <mergeCell ref="AH26:AH27"/>
-    <mergeCell ref="AI26:AI27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="H27:L27"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="AA27:AE27"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="AA24:AE24"/>
-    <mergeCell ref="AH24:AH25"/>
-    <mergeCell ref="AI24:AI25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="H25:L25"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="AA25:AE25"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="T28:T30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="W30:X30"/>
-    <mergeCell ref="AA30:AE30"/>
-    <mergeCell ref="AH30:AH31"/>
-    <mergeCell ref="AI30:AI31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="W31:X31"/>
-    <mergeCell ref="AA31:AE31"/>
-    <mergeCell ref="W28:X28"/>
-    <mergeCell ref="AA28:AE28"/>
-    <mergeCell ref="AH28:AH29"/>
-    <mergeCell ref="AI28:AI29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="W29:X29"/>
-    <mergeCell ref="AA29:AE29"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="O32:O33"/>
-    <mergeCell ref="P32:P33"/>
-    <mergeCell ref="T32:T34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="H34:L34"/>
-    <mergeCell ref="O34:O35"/>
-    <mergeCell ref="P34:P35"/>
-    <mergeCell ref="W34:X34"/>
-    <mergeCell ref="AA34:AE34"/>
-    <mergeCell ref="AH34:AH35"/>
-    <mergeCell ref="AI34:AI35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="W35:X35"/>
-    <mergeCell ref="AA35:AE35"/>
-    <mergeCell ref="W32:X32"/>
-    <mergeCell ref="AA32:AE32"/>
-    <mergeCell ref="AH32:AH33"/>
-    <mergeCell ref="AI32:AI33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="H33:L33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="AA33:AE33"/>
-    <mergeCell ref="T37:AI38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="P38:P39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="O36:O37"/>
-    <mergeCell ref="P36:P37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="O40:O41"/>
-    <mergeCell ref="P40:P41"/>
-    <mergeCell ref="T40:T42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="P42:P43"/>
-    <mergeCell ref="AI42:AI43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="W43:X43"/>
-    <mergeCell ref="AA43:AE43"/>
-    <mergeCell ref="W40:X40"/>
-    <mergeCell ref="AA40:AE40"/>
-    <mergeCell ref="AH40:AH41"/>
-    <mergeCell ref="AI40:AI41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="H41:L41"/>
-    <mergeCell ref="W41:X41"/>
-    <mergeCell ref="AA41:AE41"/>
-    <mergeCell ref="P44:P45"/>
-    <mergeCell ref="T44:T46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="H46:L46"/>
-    <mergeCell ref="O46:O47"/>
-    <mergeCell ref="P46:P47"/>
-    <mergeCell ref="W42:X42"/>
-    <mergeCell ref="AA42:AE42"/>
-    <mergeCell ref="AH42:AH43"/>
-    <mergeCell ref="U2:AH3"/>
-    <mergeCell ref="B49:F50"/>
-    <mergeCell ref="B13:N13"/>
-    <mergeCell ref="T13:AG13"/>
-    <mergeCell ref="W46:X46"/>
-    <mergeCell ref="AA46:AE46"/>
-    <mergeCell ref="AH46:AH47"/>
-    <mergeCell ref="AI46:AI47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="H47:L47"/>
-    <mergeCell ref="W47:X47"/>
-    <mergeCell ref="AA47:AE47"/>
-    <mergeCell ref="W44:X44"/>
-    <mergeCell ref="AA44:AE44"/>
-    <mergeCell ref="AH44:AH45"/>
-    <mergeCell ref="AI44:AI45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="H45:L45"/>
-    <mergeCell ref="W45:X45"/>
-    <mergeCell ref="AA45:AE45"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="H44:L44"/>
-    <mergeCell ref="O44:O45"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="T16:T18"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="C2:O3"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="U5:X5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="U4:X4"/>
+    <mergeCell ref="U12:X12"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="U8:X8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="U9:X9"/>
+    <mergeCell ref="U10:X10"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.41" right="0.5" top="0.36000000000000021" bottom="0.31000000000000005" header="0.32" footer="0.31000000000000005"/>

</xml_diff>